<commit_message>
Add more test data and first assertion.
</commit_message>
<xml_diff>
--- a/db/tests/mock_data.xlsx
+++ b/db/tests/mock_data.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="bioqc_selected_samples" sheetId="1" r:id="rId1"/>
     <sheet name="bioqc_tissue_set" sheetId="2" r:id="rId2"/>
     <sheet name="bioqc_signatures" sheetId="3" r:id="rId3"/>
-    <sheet name="bioqc_res_tissue" sheetId="4" r:id="rId4"/>
+    <sheet name="bioqc_res" sheetId="4" r:id="rId4"/>
+    <sheet name="bioqc_tissues" sheetId="6" r:id="rId5"/>
+    <sheet name="bioqc_gsm" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -73,9 +76,6 @@
     <t>homo sapiens</t>
   </si>
   <si>
-    <t>Liver</t>
-  </si>
-  <si>
     <t>liver</t>
   </si>
   <si>
@@ -94,16 +94,142 @@
     <t>tissue_set</t>
   </si>
   <si>
-    <t>fake_set</t>
-  </si>
-  <si>
     <t>intestine</t>
   </si>
   <si>
     <t>pvalue</t>
   </si>
   <si>
-    <t>second_set</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>GSM</t>
+  </si>
+  <si>
+    <t>sample 1234</t>
+  </si>
+  <si>
+    <t>sample 2222</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>SERIES_ID</t>
+  </si>
+  <si>
+    <t>GPL</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>SUBMISSION_DATE</t>
+  </si>
+  <si>
+    <t>LAST_UPDATE_DATE</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>SOURCE_NAME_CH1</t>
+  </si>
+  <si>
+    <t>ORGANISM_CH1</t>
+  </si>
+  <si>
+    <t>CHARACTERISTICS_CH1</t>
+  </si>
+  <si>
+    <t>MOLECULE_CH1</t>
+  </si>
+  <si>
+    <t>LABEL_CH1</t>
+  </si>
+  <si>
+    <t>TREATMENT_PROTOCOL_CH1</t>
+  </si>
+  <si>
+    <t>EXTRACT_PROTOCOL_CH1</t>
+  </si>
+  <si>
+    <t>LABEL_PROTOCOL_CH1</t>
+  </si>
+  <si>
+    <t>SOURCE_NAME_CH2</t>
+  </si>
+  <si>
+    <t>ORGANISM_CH2</t>
+  </si>
+  <si>
+    <t>CHARACTERISTICS_CH2</t>
+  </si>
+  <si>
+    <t>MOLECULE_CH2</t>
+  </si>
+  <si>
+    <t>LABEL_CH2</t>
+  </si>
+  <si>
+    <t>TREATMENT_PROTOCOL_CH2</t>
+  </si>
+  <si>
+    <t>EXTRACT_PROTOCOL_CH2</t>
+  </si>
+  <si>
+    <t>LABEL_PROTOCOL_CH2</t>
+  </si>
+  <si>
+    <t>HYB_PROTOCOL</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DATA_PROCESSING</t>
+  </si>
+  <si>
+    <t>CONTACT</t>
+  </si>
+  <si>
+    <t>SUPPLEMENTARY_FILE</t>
+  </si>
+  <si>
+    <t>DATA_ROW_COUNT</t>
+  </si>
+  <si>
+    <t>CHANNEL_COUNT</t>
+  </si>
+  <si>
+    <t>TISSUE_ORIG</t>
+  </si>
+  <si>
+    <t>gtex_solid</t>
+  </si>
+  <si>
+    <t>gtex_all</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>Colon Biopsy</t>
+  </si>
+  <si>
+    <t>GSM7777</t>
+  </si>
+  <si>
+    <t>Human primary liver</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>yet_another</t>
+  </si>
+  <si>
+    <t>sample 7777</t>
   </si>
 </sst>
 </file>
@@ -139,9 +265,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,16 +570,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -483,36 +610,56 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>2000</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>2000</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>2004</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -524,24 +671,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,10 +699,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,10 +713,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,7 +758,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -635,14 +782,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -711,6 +859,23 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>777</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -721,10 +886,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,10 +899,10 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,6 +936,207 @@
       </c>
       <c r="C4" s="1">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>777</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.0000000000000001E-30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>